<commit_message>
7.30 DB study commit
</commit_message>
<xml_diff>
--- a/조인.xlsx
+++ b/조인.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEBF6E8-B178-46AC-B766-A9D0C0638A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13D4C01-01F9-4739-AD61-1FD3FBDF544D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{140929FC-52E4-401A-BEFD-1AC1EE8ADE28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="133">
   <si>
     <t>S0001</t>
   </si>
@@ -448,6 +448,10 @@
   </si>
   <si>
     <t>SYS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,7 +548,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -571,6 +575,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA092FB-FD9F-4AFE-8F9C-2EB472EEF85A}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2065,7 +2072,7 @@
       <c r="I37" s="3">
         <v>8500</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J37" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K37" s="3" t="s">
@@ -2107,7 +2114,7 @@
       <c r="I38" s="3">
         <v>8200</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K38" s="3" t="s">
@@ -2147,7 +2154,7 @@
       <c r="I39" s="3">
         <v>6500</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="J39" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
@@ -2189,7 +2196,7 @@
       <c r="I40" s="3">
         <v>7000</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="J40" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2221,7 +2228,7 @@
       <c r="I41" s="3">
         <v>6400</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="J41" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2251,7 +2258,7 @@
       <c r="I42" s="3">
         <v>6000</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="J42" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2279,7 +2286,7 @@
       <c r="I43" s="3">
         <v>6000</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2311,7 +2318,7 @@
       <c r="I44" s="3">
         <v>6300</v>
       </c>
-      <c r="J44" s="3" t="s">
+      <c r="J44" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2341,7 +2348,7 @@
       <c r="I45" s="3">
         <v>5800</v>
       </c>
-      <c r="J45" s="3" t="s">
+      <c r="J45" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2369,7 +2376,7 @@
       <c r="I46" s="3">
         <v>5000</v>
       </c>
-      <c r="J46" s="3" t="s">
+      <c r="J46" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2399,7 +2406,7 @@
       <c r="I47" s="3">
         <v>4700</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="J47" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2429,7 +2436,7 @@
       <c r="I48" s="3">
         <v>6500</v>
       </c>
-      <c r="J48" s="3" t="s">
+      <c r="J48" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2459,7 +2466,7 @@
       <c r="I49" s="3">
         <v>4500</v>
       </c>
-      <c r="J49" s="3" t="s">
+      <c r="J49" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2489,7 +2496,7 @@
       <c r="I50" s="3">
         <v>5000</v>
       </c>
-      <c r="J50" s="3" t="s">
+      <c r="J50" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2519,7 +2526,7 @@
       <c r="I51" s="3">
         <v>4700</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="J51" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2549,7 +2556,7 @@
       <c r="I52" s="3">
         <v>7200</v>
       </c>
-      <c r="J52" s="3" t="s">
+      <c r="J52" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2579,7 +2586,7 @@
       <c r="I53" s="3">
         <v>4000</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="J53" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2609,7 +2616,7 @@
       <c r="I54" s="3">
         <v>5300</v>
       </c>
-      <c r="J54" s="3" t="s">
+      <c r="J54" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2637,7 +2644,7 @@
       <c r="I55" s="3">
         <v>6000</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="J55" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2665,8 +2672,8 @@
         <v>101</v>
       </c>
       <c r="I56" s="3"/>
-      <c r="J56" s="3" t="s">
-        <v>99</v>
+      <c r="J56" s="9" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>